<commit_message>
Fix course recommendation bug
</commit_message>
<xml_diff>
--- a/assets/Learning-Tools.xlsx
+++ b/assets/Learning-Tools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJ\Desktop\Personal\Freelance\Data Mining\data-mining\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243CA72A-3A97-47E0-B83E-05465771A3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632B49FF-67AF-492B-98FB-107ECA8C767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-3945" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">Writing </t>
-  </si>
-  <si>
     <t>beginners</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Intermediate</t>
   </si>
   <si>
-    <t xml:space="preserve">Listening </t>
-  </si>
-  <si>
     <t>Speaking</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Very Skilled</t>
+  </si>
+  <si>
+    <t>Listening</t>
+  </si>
+  <si>
+    <t>Writing</t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -180,9 +180,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -472,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,848 +490,848 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>16</v>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>